<commit_message>
con letras numeros mejor
</commit_message>
<xml_diff>
--- a/planilla.xlsx
+++ b/planilla.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\globato\Desktop\REDETERMINACION\Python\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7785"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -100,8 +95,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="0.00000000000"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +127,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -188,11 +194,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -212,8 +219,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Millares" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 4" xfId="1"/>
   </cellStyles>
@@ -273,7 +283,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -305,10 +315,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -340,7 +349,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -516,17 +524,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
@@ -540,7 +548,7 @@
     <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -581,7 +589,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>4</v>
       </c>
@@ -594,6 +602,9 @@
       <c r="D2">
         <v>1.6839</v>
       </c>
+      <c r="E2" s="10">
+        <v>0.1515145654</v>
+      </c>
       <c r="F2">
         <v>1994455.65</v>
       </c>
@@ -607,7 +618,7 @@
         <v>810029.24</v>
       </c>
       <c r="J2">
-        <v>1.877</v>
+        <v>1.8088</v>
       </c>
       <c r="K2">
         <v>2223168.39</v>
@@ -619,12 +630,12 @@
         <v>228712.73000000021</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>5</v>
       </c>
       <c r="B3" s="8">
-        <v>44805</v>
+        <v>44775</v>
       </c>
       <c r="C3">
         <v>315128.94</v>
@@ -632,6 +643,9 @@
       <c r="D3">
         <v>1.837</v>
       </c>
+      <c r="E3" s="10">
+        <v>1.3516516500000001E-2</v>
+      </c>
       <c r="F3">
         <v>578891.86</v>
       </c>
@@ -644,7 +658,7 @@
       <c r="I3">
         <v>263762.90999999997</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <v>2.0101</v>
       </c>
       <c r="K3">
@@ -657,12 +671,12 @@
         <v>54548.830000000075</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>6</v>
       </c>
-      <c r="B4" s="8">
-        <v>44835</v>
+      <c r="B4" s="9">
+        <v>45566</v>
       </c>
       <c r="C4">
         <v>5571912.2999999998</v>
@@ -670,6 +684,9 @@
       <c r="D4">
         <v>1.9442999999999999</v>
       </c>
+      <c r="E4" s="10">
+        <v>2.6151632131999999E-2</v>
+      </c>
       <c r="F4">
         <v>10833469.08</v>
       </c>
@@ -695,7 +712,7 @@
         <v>1170101.58</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>7</v>
       </c>
@@ -708,7 +725,7 @@
       <c r="D5">
         <v>2.0613000000000001</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>0.10639999999999999</v>
       </c>
       <c r="F5">
@@ -736,7 +753,7 @@
         <v>98177.329999999842</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>8</v>
       </c>
@@ -777,7 +794,7 @@
         <v>497271.73999999836</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>9</v>
       </c>
@@ -818,7 +835,7 @@
         <v>118123.75</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>10</v>
       </c>
@@ -859,7 +876,7 @@
         <v>372289.08000000007</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>11</v>
       </c>
@@ -900,7 +917,7 @@
         <v>96598.339999999851</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="C10">
         <v>21997963.359999999</v>
       </c>
@@ -933,14 +950,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
@@ -949,7 +966,7 @@
     <col min="5" max="5" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -969,7 +986,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="45.75">
       <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
@@ -989,14 +1006,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="C8" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="D14" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Primer push del codigo para automatizar reportes para la DPRPOPMIYSPG
</commit_message>
<xml_diff>
--- a/planilla.xlsx
+++ b/planilla.xlsx
@@ -98,7 +98,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="0.00000000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -220,7 +220,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="2" builtinId="3"/>
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -618,7 +618,7 @@
         <v>810029.24</v>
       </c>
       <c r="J2">
-        <v>1.8088</v>
+        <v>1.8888888800000001</v>
       </c>
       <c r="K2">
         <v>2223168.39</v>
@@ -659,7 +659,7 @@
         <v>263762.90999999997</v>
       </c>
       <c r="J3" s="1">
-        <v>2.0101</v>
+        <v>2.00002020202</v>
       </c>
       <c r="K3">
         <v>633440.68000000005</v>
@@ -700,7 +700,7 @@
         <v>5261556.79</v>
       </c>
       <c r="J4">
-        <v>2.1543000000000001</v>
+        <v>3.6514654160000002</v>
       </c>
       <c r="K4">
         <v>12003570.67</v>
@@ -726,7 +726,7 @@
         <v>2.0613000000000001</v>
       </c>
       <c r="E5" s="1">
-        <v>0.10639999999999999</v>
+        <v>2.6516510000000002</v>
       </c>
       <c r="F5">
         <v>1709230.81</v>
@@ -741,7 +741,7 @@
         <v>968257.32000000007</v>
       </c>
       <c r="J5">
-        <v>2.2860999999999998</v>
+        <v>5.5165160000000002</v>
       </c>
       <c r="K5">
         <v>1895635.06</v>
@@ -782,7 +782,7 @@
         <v>9491311.5899999999</v>
       </c>
       <c r="J6">
-        <v>2.4121000000000001</v>
+        <v>8.6516516499999998</v>
       </c>
       <c r="K6">
         <v>17062149.879999999</v>
@@ -823,7 +823,7 @@
         <v>2253117.81</v>
       </c>
       <c r="J7">
-        <v>2.5417000000000001</v>
+        <v>8.6516509999999993</v>
       </c>
       <c r="K7">
         <v>3909310.94</v>
@@ -864,7 +864,7 @@
         <v>7113051.2199999997</v>
       </c>
       <c r="J8">
-        <v>2.7029999999999998</v>
+        <v>9.6516509999999993</v>
       </c>
       <c r="K8">
         <v>11880725.09</v>
@@ -905,7 +905,7 @@
         <v>1872328.51</v>
       </c>
       <c r="J9">
-        <v>2.8058999999999998</v>
+        <v>5.3651650999999996</v>
       </c>
       <c r="K9">
         <v>3059201.42</v>

</xml_diff>